<commit_message>
Updated marks after CSFL-2
</commit_message>
<xml_diff>
--- a/Marksheet.xlsx
+++ b/Marksheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="114">
   <si>
     <t>2016-003</t>
   </si>
@@ -899,7 +899,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +945,9 @@
       <c r="C2" s="3" t="s">
         <v>113</v>
       </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -956,6 +959,9 @@
       <c r="C3">
         <v>53.5</v>
       </c>
+      <c r="D3">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -967,6 +973,9 @@
       <c r="C4">
         <v>31.5</v>
       </c>
+      <c r="D4">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -978,6 +987,9 @@
       <c r="C5">
         <v>31</v>
       </c>
+      <c r="D5">
+        <v>35.5</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -989,6 +1001,9 @@
       <c r="C6">
         <v>30.5</v>
       </c>
+      <c r="D6">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1000,6 +1015,9 @@
       <c r="C7">
         <v>30.5</v>
       </c>
+      <c r="D7">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1022,6 +1040,9 @@
       <c r="C9">
         <v>18</v>
       </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1033,6 +1054,9 @@
       <c r="C10">
         <v>17.5</v>
       </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1044,6 +1068,9 @@
       <c r="C11">
         <v>15</v>
       </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1055,6 +1082,9 @@
       <c r="C12">
         <v>13.5</v>
       </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1066,6 +1096,9 @@
       <c r="C13">
         <v>8.5</v>
       </c>
+      <c r="D13">
+        <v>33.5</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1087,6 +1120,9 @@
       </c>
       <c r="C15">
         <v>2.5</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to put formulas
</commit_message>
<xml_diff>
--- a/Marksheet.xlsx
+++ b/Marksheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="113">
   <si>
     <t>2016-003</t>
   </si>
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t xml:space="preserve">Piuli Bagchi </t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -409,7 +406,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,7 +896,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,8 +939,8 @@
       <c r="B2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>113</v>
+      <c r="C2" s="3">
+        <v>0</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -1029,6 +1026,9 @@
       <c r="C8">
         <v>25.5</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1068,8 +1068,8 @@
       <c r="C11">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>113</v>
+      <c r="D11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1109,6 +1109,9 @@
       </c>
       <c r="C14">
         <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adding some final things
</commit_message>
<xml_diff>
--- a/Marksheet.xlsx
+++ b/Marksheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
   <si>
     <t>2016-003</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t xml:space="preserve">Piuli Bagchi </t>
+  </si>
+  <si>
+    <t>Average Marks</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,9 +910,10 @@
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -931,8 +935,11 @@
       <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -946,7 +953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -960,7 +967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -974,7 +981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -988,7 +995,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1016,7 +1023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1030,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1044,7 +1051,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1072,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1086,7 +1093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1100,7 +1107,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>

</xml_diff>